<commit_message>
change dicrectory main file and test run
</commit_message>
<xml_diff>
--- a/TestResultLoginWeb/Test_Automation_Results.xlsx
+++ b/TestResultLoginWeb/Test_Automation_Results.xlsx
@@ -516,7 +516,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>20251128_133542</t>
+          <t>20251128_144516</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>20251128_133601</t>
+          <t>20251128_144534</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>20251128_133612</t>
+          <t>20251128_144547</t>
         </is>
       </c>
     </row>

</xml_diff>